<commit_message>
Project Dday - 3
</commit_message>
<xml_diff>
--- a/userCase/userCase.xlsx
+++ b/userCase/userCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GA - memory game" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Functionality</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Max. Highlighted Tiles Are 15</t>
   </si>
   <si>
-    <t>Number Of Tiles In The Title Should Equal Number Of Highlighted Tiles That Display In The Box</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -142,6 +139,18 @@
   </si>
   <si>
     <t>User story</t>
+  </si>
+  <si>
+    <t>Number Of Tiles In The Title Should Equal Number Of Highlighted Tiles That Displays In The Box</t>
+  </si>
+  <si>
+    <t>TO-DO</t>
+  </si>
+  <si>
+    <t>Identify my MVP (minimum functions needed to make my app work)</t>
+  </si>
+  <si>
+    <t>Insert the MVP and the user stories in the README.md file</t>
   </si>
 </sst>
 </file>
@@ -193,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +215,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -230,6 +245,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -240,7 +264,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -251,6 +275,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -589,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -600,20 +630,24 @@
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:5" ht="23">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19" customHeight="1">
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -623,8 +657,11 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="19" customHeight="1">
+      <c r="E2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="4"/>
       <c r="B3" s="2">
         <v>2</v>
@@ -632,8 +669,11 @@
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="19" customHeight="1">
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="2">
         <v>3</v>
@@ -642,7 +682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19" customHeight="1">
+    <row r="5" spans="1:5" ht="19" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="2">
         <v>4</v>
@@ -651,7 +691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19" customHeight="1">
+    <row r="6" spans="1:5" ht="19" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="2">
         <v>5</v>
@@ -660,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19" customHeight="1">
+    <row r="7" spans="1:5" ht="19" customHeight="1">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -671,7 +711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19" customHeight="1">
+    <row r="8" spans="1:5" ht="19" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="2">
         <v>7</v>
@@ -680,7 +720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19" customHeight="1">
+    <row r="9" spans="1:5" ht="19" customHeight="1">
       <c r="A9" s="4"/>
       <c r="B9" s="2">
         <v>8</v>
@@ -689,7 +729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19" customHeight="1">
+    <row r="10" spans="1:5" ht="19" customHeight="1">
       <c r="A10" s="4"/>
       <c r="B10" s="2">
         <v>9</v>
@@ -698,7 +738,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19" customHeight="1">
+    <row r="11" spans="1:5" ht="19" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="2">
         <v>10</v>
@@ -707,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19" customHeight="1">
+    <row r="12" spans="1:5" ht="19" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="2">
         <v>11</v>
@@ -716,7 +756,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="19" customHeight="1">
+    <row r="13" spans="1:5" ht="19" customHeight="1">
       <c r="A13" s="4"/>
       <c r="B13" s="2">
         <v>12</v>
@@ -725,7 +765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="19" customHeight="1">
+    <row r="14" spans="1:5" ht="19" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
@@ -736,7 +776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="19" customHeight="1">
+    <row r="15" spans="1:5" ht="19" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="2">
         <v>14</v>
@@ -745,7 +785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="19" customHeight="1">
+    <row r="16" spans="1:5" ht="19" customHeight="1">
       <c r="A16" s="4"/>
       <c r="B16" s="2">
         <v>15</v>
@@ -924,7 +964,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>